<commit_message>
Revisi Rekap IKM BWI
</commit_message>
<xml_diff>
--- a/IKMKecamatan.xlsx
+++ b/IKMKecamatan.xlsx
@@ -7,14 +7,16 @@
     <workbookView windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="2022" sheetId="1" r:id="rId1"/>
+    <sheet name="2021" sheetId="2" r:id="rId2"/>
+    <sheet name="2020" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1218" uniqueCount="83">
   <si>
     <t>No</t>
   </si>
@@ -270,10 +272,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -292,15 +294,69 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -314,47 +370,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -369,15 +387,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -385,17 +395,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -407,14 +409,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -422,8 +416,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,6 +426,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -445,19 +447,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -469,49 +519,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,61 +537,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,13 +555,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -619,13 +579,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -655,21 +657,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -687,18 +674,16 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -715,6 +700,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -736,18 +745,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -756,157 +758,154 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1283,13 +1282,2759 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:16">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:16">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:16">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:16">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:16">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:16">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:16">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:16">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:16">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:16">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:16">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:16">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:16">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:16">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:16">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:16">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:16">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:16">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:16">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:16">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:16">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:16">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="1:16">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:16">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:16">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:16">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A27:B27"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.7142857142857" customWidth="1"/>
+    <col min="15" max="15" width="10.1428571428571" customWidth="1"/>
+    <col min="16" max="16" width="15.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" spans="1:16">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:16">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:16">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" spans="1:16">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" spans="1:16">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" spans="1:16">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:16">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P8" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:16">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:16">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" spans="1:16">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" customHeight="1" spans="1:16">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:16">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:16">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P14" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:16">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:16">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P16" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:16">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="P17" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" customHeight="1" spans="1:16">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P18" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" customHeight="1" spans="1:16">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:16">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:16">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:16">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:16">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="1:16">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:16">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:16">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:16">
+      <c r="A27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P27" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A27:B27"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:P27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="15.7142857142857" customWidth="1"/>
+    <col min="15" max="15" width="10.1428571428571" customWidth="1"/>
+    <col min="16" max="16" width="15.7142857142857" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="30" customHeight="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Revisi IKM Skip Kecamatan Banyuwangi
</commit_message>
<xml_diff>
--- a/IKMKecamatan.xlsx
+++ b/IKMKecamatan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="149">
   <si>
     <t>No</t>
   </si>
@@ -199,10 +199,121 @@
     <t>Banyuwangi</t>
   </si>
   <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Giri</t>
+  </si>
+  <si>
+    <t>80.01</t>
+  </si>
+  <si>
+    <t>Wongsorejo</t>
+  </si>
+  <si>
+    <t>79.16</t>
+  </si>
+  <si>
+    <t>Songgon</t>
+  </si>
+  <si>
+    <t>87.88</t>
+  </si>
+  <si>
+    <t>Sempu</t>
+  </si>
+  <si>
+    <t>90.57</t>
+  </si>
+  <si>
+    <t>Kalipuro</t>
+  </si>
+  <si>
+    <t>80.99</t>
+  </si>
+  <si>
+    <t>Siliragung</t>
+  </si>
+  <si>
+    <t>94.72</t>
+  </si>
+  <si>
+    <t>Tegalsari</t>
+  </si>
+  <si>
+    <t>94.22</t>
+  </si>
+  <si>
+    <t>Licin</t>
+  </si>
+  <si>
+    <t>90.81</t>
+  </si>
+  <si>
+    <t>Blimbingsari</t>
+  </si>
+  <si>
+    <t>93.24</t>
+  </si>
+  <si>
+    <t>86.98</t>
+  </si>
+  <si>
     <t>0.27</t>
   </si>
   <si>
-    <t>75.00</t>
+    <t>77.99</t>
+  </si>
+  <si>
+    <t>81.79</t>
+  </si>
+  <si>
+    <t>88.07</t>
+  </si>
+  <si>
+    <t>91.98</t>
+  </si>
+  <si>
+    <t>0.23</t>
+  </si>
+  <si>
+    <t>0.26</t>
+  </si>
+  <si>
+    <t>63.83</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Tidak Baik</t>
+  </si>
+  <si>
+    <t>86.66</t>
+  </si>
+  <si>
+    <t>76.73</t>
+  </si>
+  <si>
+    <t>0.24</t>
+  </si>
+  <si>
+    <t>0.25</t>
+  </si>
+  <si>
+    <t>64.34</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>60.52</t>
+  </si>
+  <si>
+    <t>87.73</t>
+  </si>
+  <si>
+    <t>65.00</t>
   </si>
   <si>
     <t>C</t>
@@ -211,123 +322,6 @@
     <t>Kurang Baik</t>
   </si>
   <si>
-    <t>Giri</t>
-  </si>
-  <si>
-    <t>80.01</t>
-  </si>
-  <si>
-    <t>Wongsorejo</t>
-  </si>
-  <si>
-    <t>79.16</t>
-  </si>
-  <si>
-    <t>Songgon</t>
-  </si>
-  <si>
-    <t>87.88</t>
-  </si>
-  <si>
-    <t>Sempu</t>
-  </si>
-  <si>
-    <t>90.57</t>
-  </si>
-  <si>
-    <t>Kalipuro</t>
-  </si>
-  <si>
-    <t>80.99</t>
-  </si>
-  <si>
-    <t>Siliragung</t>
-  </si>
-  <si>
-    <t>94.72</t>
-  </si>
-  <si>
-    <t>Tegalsari</t>
-  </si>
-  <si>
-    <t>94.22</t>
-  </si>
-  <si>
-    <t>Licin</t>
-  </si>
-  <si>
-    <t>90.81</t>
-  </si>
-  <si>
-    <t>Blimbingsari</t>
-  </si>
-  <si>
-    <t>93.24</t>
-  </si>
-  <si>
-    <t>86.98</t>
-  </si>
-  <si>
-    <t>77.99</t>
-  </si>
-  <si>
-    <t>81.79</t>
-  </si>
-  <si>
-    <t>88.07</t>
-  </si>
-  <si>
-    <t>91.98</t>
-  </si>
-  <si>
-    <t>0.23</t>
-  </si>
-  <si>
-    <t>0.26</t>
-  </si>
-  <si>
-    <t>63.83</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>Tidak Baik</t>
-  </si>
-  <si>
-    <t>86.66</t>
-  </si>
-  <si>
-    <t>76.73</t>
-  </si>
-  <si>
-    <t>0.18</t>
-  </si>
-  <si>
-    <t>50.02</t>
-  </si>
-  <si>
-    <t>0.24</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>64.34</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
-    <t>60.52</t>
-  </si>
-  <si>
-    <t>87.73</t>
-  </si>
-  <si>
-    <t>65.00</t>
-  </si>
-  <si>
     <t>81.72</t>
   </si>
   <si>
@@ -376,9 +370,6 @@
     <t>79.94</t>
   </si>
   <si>
-    <t>75.04</t>
-  </si>
-  <si>
     <t>75.09</t>
   </si>
   <si>
@@ -443,9 +434,6 @@
   </si>
   <si>
     <t>81.96</t>
-  </si>
-  <si>
-    <t>75.02</t>
   </si>
   <si>
     <t>77.06</t>
@@ -483,8 +471,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -505,14 +493,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -527,6 +515,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -535,16 +530,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -558,21 +553,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
@@ -580,17 +560,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -610,11 +584,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -628,14 +602,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -643,7 +610,28 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -655,6 +643,18 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -670,7 +670,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -682,7 +688,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -694,7 +712,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -707,30 +737,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -754,13 +760,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -772,37 +802,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -814,31 +820,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,13 +855,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -920,30 +912,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
@@ -964,18 +932,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -987,130 +975,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2294,13 +2282,13 @@
         <v>60</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:16">
@@ -2308,7 +2296,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>17</v>
@@ -2344,7 +2332,7 @@
         <v>17</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>21</v>
@@ -2358,7 +2346,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>17</v>
@@ -2394,7 +2382,7 @@
         <v>17</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>21</v>
@@ -2408,7 +2396,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
@@ -2444,7 +2432,7 @@
         <v>32</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -2458,7 +2446,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
@@ -2494,7 +2482,7 @@
         <v>27</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>29</v>
@@ -2508,7 +2496,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -2544,7 +2532,7 @@
         <v>18</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>21</v>
@@ -2558,7 +2546,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2594,7 +2582,7 @@
         <v>32</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>29</v>
@@ -2608,7 +2596,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2644,7 +2632,7 @@
         <v>32</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>29</v>
@@ -2658,7 +2646,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>27</v>
@@ -2694,7 +2682,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>29</v>
@@ -2708,7 +2696,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2744,7 +2732,7 @@
         <v>32</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -2792,7 +2780,7 @@
         <v>25</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>21</v>
@@ -2816,7 +2804,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C17" sqref="C17:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -2911,13 +2899,13 @@
         <v>49</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>17</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -3067,7 +3055,7 @@
         <v>18</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>21</v>
@@ -3167,7 +3155,7 @@
         <v>27</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>21</v>
@@ -3367,7 +3355,7 @@
         <v>32</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>29</v>
@@ -3384,46 +3372,46 @@
         <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>89</v>
-      </c>
-      <c r="O12" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:16">
@@ -3567,7 +3555,7 @@
         <v>25</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>21</v>
@@ -3611,13 +3599,13 @@
         <v>49</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -3634,46 +3622,46 @@
         <v>59</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>94</v>
+        <v>60</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>95</v>
+        <v>60</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>91</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:16">
@@ -3681,49 +3669,49 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:16">
@@ -3731,49 +3719,49 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="P19" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:16">
@@ -3781,7 +3769,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
@@ -3817,7 +3805,7 @@
         <v>32</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -3831,7 +3819,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
@@ -3867,7 +3855,7 @@
         <v>27</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>29</v>
@@ -3881,49 +3869,49 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:16">
@@ -3931,7 +3919,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -3967,7 +3955,7 @@
         <v>32</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>29</v>
@@ -3981,7 +3969,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -4017,7 +4005,7 @@
         <v>32</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>29</v>
@@ -4031,7 +4019,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>27</v>
@@ -4067,7 +4055,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>29</v>
@@ -4081,7 +4069,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -4117,7 +4105,7 @@
         <v>32</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -4165,7 +4153,7 @@
         <v>18</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>21</v>
@@ -4189,7 +4177,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="C17" sqref="C17:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -4281,7 +4269,7 @@
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>18</v>
@@ -4290,7 +4278,7 @@
         <v>18</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -4340,7 +4328,7 @@
         <v>25</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>21</v>
@@ -4390,7 +4378,7 @@
         <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>21</v>
@@ -4440,7 +4428,7 @@
         <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>21</v>
@@ -4490,7 +4478,7 @@
         <v>25</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
@@ -4540,7 +4528,7 @@
         <v>25</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>21</v>
@@ -4590,7 +4578,7 @@
         <v>17</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>21</v>
@@ -4640,7 +4628,7 @@
         <v>27</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>29</v>
@@ -4690,7 +4678,7 @@
         <v>32</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>29</v>
@@ -4740,7 +4728,7 @@
         <v>18</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>21</v>
@@ -4790,7 +4778,7 @@
         <v>25</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>21</v>
@@ -4840,7 +4828,7 @@
         <v>17</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>21</v>
@@ -4890,7 +4878,7 @@
         <v>49</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>21</v>
@@ -4940,7 +4928,7 @@
         <v>25</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>21</v>
@@ -4990,7 +4978,7 @@
         <v>18</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -5040,13 +5028,13 @@
         <v>60</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:16">
@@ -5054,49 +5042,49 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>63</v>
+        <v>100</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:16">
@@ -5104,7 +5092,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>49</v>
@@ -5140,7 +5128,7 @@
         <v>17</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>21</v>
@@ -5154,7 +5142,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
@@ -5190,7 +5178,7 @@
         <v>24</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -5204,7 +5192,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>25</v>
@@ -5240,7 +5228,7 @@
         <v>25</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>29</v>
@@ -5254,7 +5242,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>17</v>
@@ -5290,7 +5278,7 @@
         <v>17</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>21</v>
@@ -5304,7 +5292,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
@@ -5340,7 +5328,7 @@
         <v>17</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>21</v>
@@ -5354,7 +5342,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>17</v>
@@ -5390,7 +5378,7 @@
         <v>25</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>21</v>
@@ -5404,7 +5392,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
@@ -5440,7 +5428,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>21</v>
@@ -5454,7 +5442,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>25</v>
@@ -5490,7 +5478,7 @@
         <v>27</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -5538,7 +5526,7 @@
         <v>24</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>21</v>
@@ -5561,8 +5549,8 @@
   <sheetPr/>
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -5654,7 +5642,7 @@
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>17</v>
@@ -5663,7 +5651,7 @@
         <v>17</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -5713,7 +5701,7 @@
         <v>27</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>21</v>
@@ -5763,7 +5751,7 @@
         <v>27</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -5813,7 +5801,7 @@
         <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>21</v>
@@ -5863,7 +5851,7 @@
         <v>24</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>21</v>
@@ -5913,7 +5901,7 @@
         <v>25</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>21</v>
@@ -5963,7 +5951,7 @@
         <v>18</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>21</v>
@@ -6013,7 +6001,7 @@
         <v>32</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>29</v>
@@ -6063,7 +6051,7 @@
         <v>25</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>29</v>
@@ -6113,7 +6101,7 @@
         <v>24</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>21</v>
@@ -6163,7 +6151,7 @@
         <v>25</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>21</v>
@@ -6213,7 +6201,7 @@
         <v>27</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>29</v>
@@ -6263,7 +6251,7 @@
         <v>17</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>21</v>
@@ -6313,7 +6301,7 @@
         <v>24</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>21</v>
@@ -6363,7 +6351,7 @@
         <v>17</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -6413,13 +6401,13 @@
         <v>60</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>142</v>
+        <v>60</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:16">
@@ -6427,7 +6415,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>49</v>
@@ -6463,7 +6451,7 @@
         <v>49</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>21</v>
@@ -6477,7 +6465,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -6513,7 +6501,7 @@
         <v>24</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>21</v>
@@ -6527,7 +6515,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
@@ -6563,7 +6551,7 @@
         <v>27</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -6577,7 +6565,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>24</v>
@@ -6613,7 +6601,7 @@
         <v>25</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>21</v>
@@ -6627,7 +6615,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>17</v>
@@ -6663,7 +6651,7 @@
         <v>17</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>21</v>
@@ -6677,7 +6665,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
@@ -6704,7 +6692,7 @@
         <v>17</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>17</v>
@@ -6713,7 +6701,7 @@
         <v>17</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>21</v>
@@ -6727,7 +6715,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -6763,7 +6751,7 @@
         <v>32</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>29</v>
@@ -6777,7 +6765,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
@@ -6813,7 +6801,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>21</v>
@@ -6827,7 +6815,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>25</v>
@@ -6863,7 +6851,7 @@
         <v>32</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -6911,7 +6899,7 @@
         <v>24</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Revisi Excel Rekap Kecamatan IKM Tanpa Banyuwangi
</commit_message>
<xml_diff>
--- a/IKMKecamatan.xlsx
+++ b/IKMKecamatan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="148">
   <si>
     <t>No</t>
   </si>
@@ -256,7 +256,7 @@
     <t>93.24</t>
   </si>
   <si>
-    <t>86.98</t>
+    <t>87.98</t>
   </si>
   <si>
     <t>0.27</t>
@@ -322,7 +322,7 @@
     <t>Kurang Baik</t>
   </si>
   <si>
-    <t>81.72</t>
+    <t>84.37</t>
   </si>
   <si>
     <t>82.04</t>
@@ -397,9 +397,6 @@
     <t>89.49</t>
   </si>
   <si>
-    <t>83.64</t>
-  </si>
-  <si>
     <t>80.46</t>
   </si>
   <si>
@@ -463,7 +460,7 @@
     <t>90.73</t>
   </si>
   <si>
-    <t>84.90</t>
+    <t>85.72</t>
   </si>
 </sst>
 </file>
@@ -471,10 +468,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -493,11 +490,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -515,13 +512,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -530,16 +520,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -554,7 +545,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -569,18 +575,18 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -592,9 +598,29 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -603,35 +629,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -652,7 +649,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -664,7 +763,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -676,7 +775,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -688,103 +811,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -796,37 +823,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -855,17 +852,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -885,11 +876,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -911,9 +908,29 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -932,26 +949,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -960,145 +957,145 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2747,25 +2744,25 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>24</v>
@@ -2774,7 +2771,7 @@
         <v>25</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>25</v>
@@ -2804,7 +2801,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:P17"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -4120,37 +4117,37 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="N27" s="1" t="s">
         <v>101</v>
@@ -4177,7 +4174,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:P17"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -5502,7 +5499,7 @@
         <v>18</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>18</v>
@@ -5526,7 +5523,7 @@
         <v>24</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>21</v>
@@ -5549,8 +5546,8 @@
   <sheetPr/>
   <dimension ref="A1:P27"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -5651,7 +5648,7 @@
         <v>17</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -5701,7 +5698,7 @@
         <v>27</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>21</v>
@@ -5751,7 +5748,7 @@
         <v>27</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -5801,7 +5798,7 @@
         <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>21</v>
@@ -5851,7 +5848,7 @@
         <v>24</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>21</v>
@@ -5901,7 +5898,7 @@
         <v>25</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>21</v>
@@ -6001,7 +5998,7 @@
         <v>32</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>29</v>
@@ -6051,7 +6048,7 @@
         <v>25</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>29</v>
@@ -6101,7 +6098,7 @@
         <v>24</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>21</v>
@@ -6201,7 +6198,7 @@
         <v>27</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>29</v>
@@ -6251,7 +6248,7 @@
         <v>17</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>21</v>
@@ -6301,7 +6298,7 @@
         <v>24</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>21</v>
@@ -6351,7 +6348,7 @@
         <v>17</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -6451,7 +6448,7 @@
         <v>49</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>21</v>
@@ -6501,7 +6498,7 @@
         <v>24</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>21</v>
@@ -6551,7 +6548,7 @@
         <v>27</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -6601,7 +6598,7 @@
         <v>25</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>21</v>
@@ -6651,7 +6648,7 @@
         <v>17</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>21</v>
@@ -6701,7 +6698,7 @@
         <v>17</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>21</v>
@@ -6751,7 +6748,7 @@
         <v>32</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>29</v>
@@ -6801,7 +6798,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>21</v>
@@ -6851,7 +6848,7 @@
         <v>32</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -6872,16 +6869,16 @@
         <v>24</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>24</v>
@@ -6896,10 +6893,10 @@
         <v>24</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Revisi Rekap Survei IKM Non Kelurahan Series
</commit_message>
<xml_diff>
--- a/IKMKecamatan.xlsx
+++ b/IKMKecamatan.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1624" uniqueCount="145">
   <si>
     <t>No</t>
   </si>
@@ -193,7 +193,7 @@
     <t>Glagah</t>
   </si>
   <si>
-    <t>84.80</t>
+    <t>88.34</t>
   </si>
   <si>
     <t>Banyuwangi</t>
@@ -205,9 +205,6 @@
     <t>Giri</t>
   </si>
   <si>
-    <t>80.01</t>
-  </si>
-  <si>
     <t>Wongsorejo</t>
   </si>
   <si>
@@ -229,7 +226,7 @@
     <t>Kalipuro</t>
   </si>
   <si>
-    <t>80.99</t>
+    <t>91.96</t>
   </si>
   <si>
     <t>Siliragung</t>
@@ -256,7 +253,7 @@
     <t>93.24</t>
   </si>
   <si>
-    <t>87.98</t>
+    <t>89.65</t>
   </si>
   <si>
     <t>0.27</t>
@@ -292,162 +289,156 @@
     <t>86.66</t>
   </si>
   <si>
-    <t>76.73</t>
-  </si>
-  <si>
-    <t>0.24</t>
+    <t>85.95</t>
+  </si>
+  <si>
+    <t>0.22</t>
+  </si>
+  <si>
+    <t>60.52</t>
+  </si>
+  <si>
+    <t>87.73</t>
+  </si>
+  <si>
+    <t>90.92</t>
+  </si>
+  <si>
+    <t>88.62</t>
+  </si>
+  <si>
+    <t>82.04</t>
+  </si>
+  <si>
+    <t>87.10</t>
+  </si>
+  <si>
+    <t>87.59</t>
+  </si>
+  <si>
+    <t>85.38</t>
+  </si>
+  <si>
+    <t>88.59</t>
+  </si>
+  <si>
+    <t>84.54</t>
+  </si>
+  <si>
+    <t>78.46</t>
+  </si>
+  <si>
+    <t>91.91</t>
+  </si>
+  <si>
+    <t>92.55</t>
+  </si>
+  <si>
+    <t>83.14</t>
+  </si>
+  <si>
+    <t>88.27</t>
+  </si>
+  <si>
+    <t>80.07</t>
+  </si>
+  <si>
+    <t>77.75</t>
+  </si>
+  <si>
+    <t>86.75</t>
+  </si>
+  <si>
+    <t>81.13</t>
+  </si>
+  <si>
+    <t>75.25</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Kurang Baik</t>
+  </si>
+  <si>
+    <t>78.06</t>
+  </si>
+  <si>
+    <t>82.22</t>
+  </si>
+  <si>
+    <t>89.37</t>
+  </si>
+  <si>
+    <t>80.41</t>
+  </si>
+  <si>
+    <t>84.13</t>
+  </si>
+  <si>
+    <t>88.08</t>
+  </si>
+  <si>
+    <t>89.49</t>
+  </si>
+  <si>
+    <t>84.82</t>
+  </si>
+  <si>
+    <t>80.46</t>
+  </si>
+  <si>
+    <t>87.76</t>
+  </si>
+  <si>
+    <t>88.57</t>
+  </si>
+  <si>
+    <t>84.65</t>
+  </si>
+  <si>
+    <t>84.76</t>
+  </si>
+  <si>
+    <t>85.33</t>
+  </si>
+  <si>
+    <t>90.82</t>
+  </si>
+  <si>
+    <t>93.02</t>
+  </si>
+  <si>
+    <t>85.46</t>
+  </si>
+  <si>
+    <t>79.95</t>
+  </si>
+  <si>
+    <t>84.61</t>
+  </si>
+  <si>
+    <t>83.10</t>
+  </si>
+  <si>
+    <t>80.85</t>
+  </si>
+  <si>
+    <t>84.05</t>
+  </si>
+  <si>
+    <t>86.81</t>
+  </si>
+  <si>
+    <t>88.24</t>
+  </si>
+  <si>
+    <t>84.14</t>
   </si>
   <si>
     <t>0.25</t>
   </si>
   <si>
-    <t>64.34</t>
-  </si>
-  <si>
-    <t>0.22</t>
-  </si>
-  <si>
-    <t>60.52</t>
-  </si>
-  <si>
-    <t>87.73</t>
-  </si>
-  <si>
-    <t>65.00</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
-    <t>Kurang Baik</t>
-  </si>
-  <si>
-    <t>84.37</t>
-  </si>
-  <si>
-    <t>82.04</t>
-  </si>
-  <si>
-    <t>87.10</t>
-  </si>
-  <si>
-    <t>87.59</t>
-  </si>
-  <si>
-    <t>85.38</t>
-  </si>
-  <si>
-    <t>88.59</t>
-  </si>
-  <si>
-    <t>84.54</t>
-  </si>
-  <si>
-    <t>78.46</t>
-  </si>
-  <si>
-    <t>91.91</t>
-  </si>
-  <si>
-    <t>92.55</t>
-  </si>
-  <si>
-    <t>83.14</t>
-  </si>
-  <si>
-    <t>88.27</t>
-  </si>
-  <si>
-    <t>80.07</t>
-  </si>
-  <si>
-    <t>77.75</t>
-  </si>
-  <si>
-    <t>86.75</t>
-  </si>
-  <si>
-    <t>79.94</t>
-  </si>
-  <si>
-    <t>75.09</t>
-  </si>
-  <si>
-    <t>78.06</t>
-  </si>
-  <si>
-    <t>82.22</t>
-  </si>
-  <si>
-    <t>89.37</t>
-  </si>
-  <si>
-    <t>81.28</t>
-  </si>
-  <si>
-    <t>80.41</t>
-  </si>
-  <si>
-    <t>84.13</t>
-  </si>
-  <si>
-    <t>88.08</t>
-  </si>
-  <si>
-    <t>89.49</t>
-  </si>
-  <si>
-    <t>80.46</t>
-  </si>
-  <si>
-    <t>87.76</t>
-  </si>
-  <si>
-    <t>88.57</t>
-  </si>
-  <si>
-    <t>84.65</t>
-  </si>
-  <si>
-    <t>84.76</t>
-  </si>
-  <si>
-    <t>85.33</t>
-  </si>
-  <si>
-    <t>90.82</t>
-  </si>
-  <si>
-    <t>93.02</t>
-  </si>
-  <si>
-    <t>85.46</t>
-  </si>
-  <si>
-    <t>79.95</t>
-  </si>
-  <si>
-    <t>84.61</t>
-  </si>
-  <si>
-    <t>81.96</t>
-  </si>
-  <si>
-    <t>77.06</t>
-  </si>
-  <si>
-    <t>84.05</t>
-  </si>
-  <si>
-    <t>86.81</t>
-  </si>
-  <si>
-    <t>88.24</t>
-  </si>
-  <si>
-    <t>80.34</t>
-  </si>
-  <si>
     <t>78.62</t>
   </si>
   <si>
@@ -460,7 +451,7 @@
     <t>90.73</t>
   </si>
   <si>
-    <t>85.72</t>
+    <t>86.20</t>
   </si>
 </sst>
 </file>
@@ -469,8 +460,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="21">
@@ -490,16 +481,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -512,25 +496,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -544,8 +533,71 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,45 +612,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -606,29 +619,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -643,13 +634,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,19 +796,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -685,139 +808,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -852,15 +843,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -876,17 +858,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -908,29 +884,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -949,21 +905,56 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -972,130 +963,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2196,46 +2187,46 @@
         <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="N16" s="1" t="s">
         <v>58</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:16">
@@ -2296,46 +2287,46 @@
         <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:16">
@@ -2343,43 +2334,43 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N19" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>64</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>21</v>
@@ -2393,7 +2384,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
@@ -2429,7 +2420,7 @@
         <v>32</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -2443,7 +2434,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
@@ -2479,7 +2470,7 @@
         <v>27</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>29</v>
@@ -2493,49 +2484,49 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>70</v>
-      </c>
       <c r="O22" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:16">
@@ -2543,7 +2534,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -2579,7 +2570,7 @@
         <v>32</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>29</v>
@@ -2593,7 +2584,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -2629,7 +2620,7 @@
         <v>32</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>29</v>
@@ -2643,7 +2634,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>27</v>
@@ -2679,7 +2670,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>29</v>
@@ -2693,7 +2684,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -2729,7 +2720,7 @@
         <v>32</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -2753,10 +2744,10 @@
         <v>25</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>25</v>
@@ -2765,25 +2756,25 @@
         <v>25</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>25</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -2896,13 +2887,13 @@
         <v>49</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -3052,7 +3043,7 @@
         <v>18</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>21</v>
@@ -3152,7 +3143,7 @@
         <v>27</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>21</v>
@@ -3352,7 +3343,7 @@
         <v>32</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>29</v>
@@ -3369,46 +3360,46 @@
         <v>48</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="N12" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="N12" s="1" t="s">
+      <c r="O12" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="P12" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:16">
@@ -3552,7 +3543,7 @@
         <v>25</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>21</v>
@@ -3569,40 +3560,40 @@
         <v>57</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>80</v>
+        <v>18</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -3669,46 +3660,46 @@
         <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>92</v>
+        <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>93</v>
+        <v>26</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>85</v>
+        <v>24</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>88</v>
+        <v>29</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>89</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:16">
@@ -3716,49 +3707,49 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="M19" s="1" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="O19" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="P19" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:16">
@@ -3766,7 +3757,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
@@ -3802,7 +3793,7 @@
         <v>32</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -3816,7 +3807,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
@@ -3852,7 +3843,7 @@
         <v>27</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>29</v>
@@ -3866,49 +3857,49 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>93</v>
+        <v>19</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>85</v>
+        <v>27</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>85</v>
+        <v>25</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>99</v>
+        <v>29</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>100</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:16">
@@ -3916,7 +3907,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>32</v>
@@ -3952,7 +3943,7 @@
         <v>32</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>29</v>
@@ -3966,7 +3957,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -4002,7 +3993,7 @@
         <v>32</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>29</v>
@@ -4016,7 +4007,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>27</v>
@@ -4052,7 +4043,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>29</v>
@@ -4066,7 +4057,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>32</v>
@@ -4102,7 +4093,7 @@
         <v>32</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -4117,46 +4108,46 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="M27" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="P27" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -4266,7 +4257,7 @@
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>18</v>
@@ -4275,7 +4266,7 @@
         <v>18</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -4325,7 +4316,7 @@
         <v>25</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>21</v>
@@ -4375,7 +4366,7 @@
         <v>25</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>21</v>
@@ -4425,7 +4416,7 @@
         <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>21</v>
@@ -4475,7 +4466,7 @@
         <v>25</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>29</v>
@@ -4525,7 +4516,7 @@
         <v>25</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>21</v>
@@ -4575,7 +4566,7 @@
         <v>17</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>21</v>
@@ -4625,7 +4616,7 @@
         <v>27</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>29</v>
@@ -4675,7 +4666,7 @@
         <v>32</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>29</v>
@@ -4725,7 +4716,7 @@
         <v>18</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>21</v>
@@ -4775,7 +4766,7 @@
         <v>25</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>21</v>
@@ -4825,7 +4816,7 @@
         <v>17</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>21</v>
@@ -4875,7 +4866,7 @@
         <v>49</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>21</v>
@@ -4925,7 +4916,7 @@
         <v>25</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>21</v>
@@ -4960,13 +4951,13 @@
         <v>17</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>17</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>17</v>
@@ -4975,7 +4966,7 @@
         <v>18</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -5042,46 +5033,46 @@
         <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:16">
@@ -5089,7 +5080,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>49</v>
@@ -5125,7 +5116,7 @@
         <v>17</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>21</v>
@@ -5139,7 +5130,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>17</v>
@@ -5175,7 +5166,7 @@
         <v>24</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -5189,7 +5180,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>25</v>
@@ -5225,7 +5216,7 @@
         <v>25</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>29</v>
@@ -5239,43 +5230,43 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>21</v>
@@ -5289,7 +5280,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
@@ -5325,7 +5316,7 @@
         <v>17</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>21</v>
@@ -5339,7 +5330,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>17</v>
@@ -5375,7 +5366,7 @@
         <v>25</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>21</v>
@@ -5389,7 +5380,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
@@ -5425,7 +5416,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>21</v>
@@ -5439,7 +5430,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>25</v>
@@ -5475,7 +5466,7 @@
         <v>27</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -5490,10 +5481,10 @@
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>18</v>
@@ -5508,7 +5499,7 @@
         <v>18</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>18</v>
@@ -5517,13 +5508,13 @@
         <v>24</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="M27" s="1" t="s">
         <v>24</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>21</v>
@@ -5639,7 +5630,7 @@
         <v>17</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>17</v>
@@ -5648,7 +5639,7 @@
         <v>17</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>21</v>
@@ -5698,7 +5689,7 @@
         <v>27</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>21</v>
@@ -5748,7 +5739,7 @@
         <v>27</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O4" s="1" t="s">
         <v>29</v>
@@ -5798,7 +5789,7 @@
         <v>25</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>21</v>
@@ -5848,7 +5839,7 @@
         <v>24</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="O6" s="1" t="s">
         <v>21</v>
@@ -5898,7 +5889,7 @@
         <v>25</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>21</v>
@@ -5948,7 +5939,7 @@
         <v>18</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="O8" s="1" t="s">
         <v>21</v>
@@ -5998,7 +5989,7 @@
         <v>32</v>
       </c>
       <c r="N9" s="1" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>29</v>
@@ -6048,7 +6039,7 @@
         <v>25</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>29</v>
@@ -6098,7 +6089,7 @@
         <v>24</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>21</v>
@@ -6148,7 +6139,7 @@
         <v>25</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="O12" s="1" t="s">
         <v>21</v>
@@ -6198,7 +6189,7 @@
         <v>27</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="O13" s="1" t="s">
         <v>29</v>
@@ -6248,7 +6239,7 @@
         <v>17</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="O14" s="1" t="s">
         <v>21</v>
@@ -6298,7 +6289,7 @@
         <v>24</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>21</v>
@@ -6324,19 +6315,19 @@
         <v>18</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>18</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>18</v>
@@ -6345,10 +6336,10 @@
         <v>18</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="O16" s="1" t="s">
         <v>21</v>
@@ -6415,40 +6406,40 @@
         <v>61</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="O18" s="1" t="s">
         <v>21</v>
@@ -6462,7 +6453,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -6498,7 +6489,7 @@
         <v>24</v>
       </c>
       <c r="N19" s="1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="O19" s="1" t="s">
         <v>21</v>
@@ -6512,7 +6503,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>24</v>
@@ -6548,7 +6539,7 @@
         <v>27</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="O20" s="1" t="s">
         <v>21</v>
@@ -6562,7 +6553,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>24</v>
@@ -6598,7 +6589,7 @@
         <v>25</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="O21" s="1" t="s">
         <v>21</v>
@@ -6612,43 +6603,43 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="O22" s="1" t="s">
         <v>21</v>
@@ -6662,7 +6653,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>17</v>
@@ -6689,7 +6680,7 @@
         <v>17</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
       <c r="L23" s="1" t="s">
         <v>17</v>
@@ -6698,7 +6689,7 @@
         <v>17</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="O23" s="1" t="s">
         <v>21</v>
@@ -6712,7 +6703,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>32</v>
@@ -6748,7 +6739,7 @@
         <v>32</v>
       </c>
       <c r="N24" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>29</v>
@@ -6762,7 +6753,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>25</v>
@@ -6798,7 +6789,7 @@
         <v>27</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>21</v>
@@ -6812,7 +6803,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>25</v>
@@ -6848,7 +6839,7 @@
         <v>32</v>
       </c>
       <c r="N26" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="O26" s="1" t="s">
         <v>29</v>
@@ -6884,10 +6875,10 @@
         <v>24</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L27" s="1" t="s">
         <v>24</v>
@@ -6896,7 +6887,7 @@
         <v>25</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="O27" s="1" t="s">
         <v>21</v>

</xml_diff>